<commit_message>
Stock Card Report - template update
</commit_message>
<xml_diff>
--- a/public/excel_templates/stock-card-report-template-lo.xlsx
+++ b/public/excel_templates/stock-card-report-template-lo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Unlimited Network of Opportunities International Corp.</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>TIN: 006-505-014 VAT</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Subgroup</t>
   </si>
 </sst>
 </file>
@@ -393,34 +399,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -430,8 +438,10 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -442,22 +452,28 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -467,8 +483,10 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -478,6 +496,8 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>